<commit_message>
Adding data to example Excel.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A49CDA-5C51-6642-839C-79BA03B2997E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCEA5ED-9303-D942-B1F4-CFF367C79B16}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="127">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -96,9 +96,6 @@
     <t>EXTENSIONID</t>
   </si>
   <si>
-    <t>extensiontest</t>
-  </si>
-  <si>
     <t>STARTDATE</t>
   </si>
   <si>
@@ -121,6 +118,297 @@
   </si>
   <si>
     <t>2018-12-31</t>
+  </si>
+  <si>
+    <t>testcode02</t>
+  </si>
+  <si>
+    <t>testcode03</t>
+  </si>
+  <si>
+    <t>testcode04</t>
+  </si>
+  <si>
+    <t>testcode05</t>
+  </si>
+  <si>
+    <t>testcode06</t>
+  </si>
+  <si>
+    <t>testcode07</t>
+  </si>
+  <si>
+    <t>testcode08</t>
+  </si>
+  <si>
+    <t>testcode09</t>
+  </si>
+  <si>
+    <t>testcode10</t>
+  </si>
+  <si>
+    <t>Testikoodi 02</t>
+  </si>
+  <si>
+    <t>Test code 02</t>
+  </si>
+  <si>
+    <t>Testikoodi 03</t>
+  </si>
+  <si>
+    <t>Test code 03</t>
+  </si>
+  <si>
+    <t>Testikoodi 04</t>
+  </si>
+  <si>
+    <t>Test code 04</t>
+  </si>
+  <si>
+    <t>Testikoodi 05</t>
+  </si>
+  <si>
+    <t>Test code 05</t>
+  </si>
+  <si>
+    <t>Testikoodi 06</t>
+  </si>
+  <si>
+    <t>Test code 06</t>
+  </si>
+  <si>
+    <t>Testikoodi 07</t>
+  </si>
+  <si>
+    <t>Test code 07</t>
+  </si>
+  <si>
+    <t>Testikoodi 08</t>
+  </si>
+  <si>
+    <t>Test code 08</t>
+  </si>
+  <si>
+    <t>Testikoodi 09</t>
+  </si>
+  <si>
+    <t>Test code 09</t>
+  </si>
+  <si>
+    <t>Testikoodi 10</t>
+  </si>
+  <si>
+    <t>Test code 10</t>
+  </si>
+  <si>
+    <t>testcode11</t>
+  </si>
+  <si>
+    <t>Testikoodi 11</t>
+  </si>
+  <si>
+    <t>Test code 11</t>
+  </si>
+  <si>
+    <t>testcode12</t>
+  </si>
+  <si>
+    <t>Testikoodi 12</t>
+  </si>
+  <si>
+    <t>Test code 12</t>
+  </si>
+  <si>
+    <t>testcode13</t>
+  </si>
+  <si>
+    <t>Testikoodi 13</t>
+  </si>
+  <si>
+    <t>Test code 13</t>
+  </si>
+  <si>
+    <t>testcode14</t>
+  </si>
+  <si>
+    <t>Testikoodi 14</t>
+  </si>
+  <si>
+    <t>Test code 14</t>
+  </si>
+  <si>
+    <t>testcode15</t>
+  </si>
+  <si>
+    <t>Testikoodi 15</t>
+  </si>
+  <si>
+    <t>Test code 15</t>
+  </si>
+  <si>
+    <t>testcode16</t>
+  </si>
+  <si>
+    <t>Testikoodi 16</t>
+  </si>
+  <si>
+    <t>Test code 16</t>
+  </si>
+  <si>
+    <t>testcode17</t>
+  </si>
+  <si>
+    <t>Testikoodi 17</t>
+  </si>
+  <si>
+    <t>Test code 17</t>
+  </si>
+  <si>
+    <t>testcode18</t>
+  </si>
+  <si>
+    <t>Testikoodi 18</t>
+  </si>
+  <si>
+    <t>Test code 18</t>
+  </si>
+  <si>
+    <t>testcode19</t>
+  </si>
+  <si>
+    <t>Testikoodi 19</t>
+  </si>
+  <si>
+    <t>Test code 19</t>
+  </si>
+  <si>
+    <t>testcode20</t>
+  </si>
+  <si>
+    <t>testcode21</t>
+  </si>
+  <si>
+    <t>testcode22</t>
+  </si>
+  <si>
+    <t>testcode23</t>
+  </si>
+  <si>
+    <t>testcode24</t>
+  </si>
+  <si>
+    <t>testcode25</t>
+  </si>
+  <si>
+    <t>extensiontest1</t>
+  </si>
+  <si>
+    <t>extensiontest2</t>
+  </si>
+  <si>
+    <t>extensiontest3</t>
+  </si>
+  <si>
+    <t>extensiontest4</t>
+  </si>
+  <si>
+    <t>extensiontest5</t>
+  </si>
+  <si>
+    <t>extensiontest6</t>
+  </si>
+  <si>
+    <t>extensiontest7</t>
+  </si>
+  <si>
+    <t>extensiontest8</t>
+  </si>
+  <si>
+    <t>extensiontest9</t>
+  </si>
+  <si>
+    <t>extensiontest10</t>
+  </si>
+  <si>
+    <t>extensiontest11</t>
+  </si>
+  <si>
+    <t>extensiontest12</t>
+  </si>
+  <si>
+    <t>extensiontest13</t>
+  </si>
+  <si>
+    <t>extensiontest14</t>
+  </si>
+  <si>
+    <t>extensiontest15</t>
+  </si>
+  <si>
+    <t>extensiontest16</t>
+  </si>
+  <si>
+    <t>extensiontest17</t>
+  </si>
+  <si>
+    <t>extensiontest18</t>
+  </si>
+  <si>
+    <t>extensiontest19</t>
+  </si>
+  <si>
+    <t>extensiontest20</t>
+  </si>
+  <si>
+    <t>extensiontest21</t>
+  </si>
+  <si>
+    <t>extensiontest22</t>
+  </si>
+  <si>
+    <t>extensiontest23</t>
+  </si>
+  <si>
+    <t>extensiontest24</t>
+  </si>
+  <si>
+    <t>extensiontest25</t>
+  </si>
+  <si>
+    <t>Testikoodi 20</t>
+  </si>
+  <si>
+    <t>Test code 20</t>
+  </si>
+  <si>
+    <t>Testikoodi 21</t>
+  </si>
+  <si>
+    <t>Test code 21</t>
+  </si>
+  <si>
+    <t>Testikoodi 22</t>
+  </si>
+  <si>
+    <t>Test code 22</t>
+  </si>
+  <si>
+    <t>Testikoodi 23</t>
+  </si>
+  <si>
+    <t>Test code 23</t>
+  </si>
+  <si>
+    <t>Testikoodi 24</t>
+  </si>
+  <si>
+    <t>Test code 24</t>
+  </si>
+  <si>
+    <t>Testikoodi 25</t>
+  </si>
+  <si>
+    <t>Test code 25</t>
   </si>
 </sst>
 </file>
@@ -498,13 +786,13 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -516,10 +804,10 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -530,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -542,10 +830,10 @@
         <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -556,10 +844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898AAFE0-BD98-4D41-8F23-B5EFB1CF0430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,6 +884,342 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -605,7 +1229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4460C0-3790-E444-9C90-6BF5633E17FB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -635,10 +1259,10 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -658,10 +1282,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -671,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F821AE-14EF-9447-94FD-816F31696438}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,13 +1325,277 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring to use order instead of extensionOrder.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCEA5ED-9303-D942-B1F4-CFF367C79B16}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBB2595-B777-E84A-8FA1-432B774D799D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -93,9 +93,6 @@
     <t>CODE</t>
   </si>
   <si>
-    <t>EXTENSIONID</t>
-  </si>
-  <si>
     <t>STARTDATE</t>
   </si>
   <si>
@@ -336,9 +333,6 @@
     <t>extensiontest12</t>
   </si>
   <si>
-    <t>extensiontest13</t>
-  </si>
-  <si>
     <t>extensiontest14</t>
   </si>
   <si>
@@ -409,6 +403,9 @@
   </si>
   <si>
     <t>Test code 25</t>
+  </si>
+  <si>
+    <t>RELATION</t>
   </si>
 </sst>
 </file>
@@ -764,7 +761,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,13 +783,13 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -804,10 +801,10 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -818,7 +815,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -830,10 +827,10 @@
         <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898AAFE0-BD98-4D41-8F23-B5EFB1CF0430}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -886,338 +883,338 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
         <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
         <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
         <v>53</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>64</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>66</v>
       </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>70</v>
-      </c>
-      <c r="D16" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>73</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
         <v>78</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>79</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
         <v>81</v>
       </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>82</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1230,7 +1227,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,10 +1256,10 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1282,10 +1279,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1297,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F821AE-14EF-9447-94FD-816F31696438}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1320,12 +1317,12 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1336,266 +1333,302 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extension relation and deletion implementation fixes.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBB2595-B777-E84A-8FA1-432B774D799D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDFEA0C-481E-E24A-9F32-19208C67C708}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="126">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -87,9 +87,6 @@
     <t>EXTENSIONVALUE</t>
   </si>
   <si>
-    <t>EXTENSIONORDER</t>
-  </si>
-  <si>
     <t>CODE</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>RELATION</t>
+  </si>
+  <si>
+    <t>ORDER</t>
   </si>
 </sst>
 </file>
@@ -783,13 +783,13 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -801,10 +801,10 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -815,7 +815,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -827,10 +827,10 @@
         <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -841,380 +841,458 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898AAFE0-BD98-4D41-8F23-B5EFB1CF0430}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>57</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>59</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>60</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>63</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
         <v>65</v>
       </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>66</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>69</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>72</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
         <v>74</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>75</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>78</v>
       </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
         <v>80</v>
       </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>81</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="E22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>84</v>
       </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="E23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>85</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="E24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>86</v>
       </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="E25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>87</v>
       </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>123</v>
-      </c>
-      <c r="D26" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1256,10 +1334,10 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1279,10 +1357,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1294,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F821AE-14EF-9447-94FD-816F31696438}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1311,18 +1389,18 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1333,302 +1411,338 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ExtensionScheme datamodel related refactoring, dynamic Excel sheet names.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDFEA0C-481E-E24A-9F32-19208C67C708}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66B09ED-5AA6-DD42-85AC-7BD25142CE58}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
-    <sheet name="Codes" sheetId="2" r:id="rId2"/>
-    <sheet name="ExtensionSchemes" sheetId="3" r:id="rId3"/>
+    <sheet name="Codes_exttest1" sheetId="2" r:id="rId2"/>
+    <sheet name="ExtensionSchemes_exttest1" sheetId="3" r:id="rId3"/>
     <sheet name="Extensions_test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -406,6 +406,24 @@
   </si>
   <si>
     <t>ORDER</t>
+  </si>
+  <si>
+    <t>EXTENSIONSCHEMESSHEET</t>
+  </si>
+  <si>
+    <t>CODESSHEET</t>
+  </si>
+  <si>
+    <t>EXTENSIONSSHEET</t>
+  </si>
+  <si>
+    <t>Codes_exttest1</t>
+  </si>
+  <si>
+    <t>ExtensionSchemes_exttest1</t>
+  </si>
+  <si>
+    <t>Extensions_test</t>
   </si>
 </sst>
 </file>
@@ -758,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3255037-6CC6-5342-A480-CDB6C5B76D51}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,9 +791,10 @@
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -806,8 +825,14 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -831,6 +856,12 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -843,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898AAFE0-BD98-4D41-8F23-B5EFB1CF0430}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1302,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4460C0-3790-E444-9C90-6BF5633E17FB}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1317,7 +1348,7 @@
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1339,8 +1370,11 @@
       <c r="G1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1361,6 +1395,9 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing integration test Excel regarding hierarchy limit for extensions.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66B09ED-5AA6-DD42-85AC-7BD25142CE58}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62E2618-C61F-1644-BD82-9B7DE3F8E372}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="7060" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="31540" activeTab="3" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="132">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -1335,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4460C0-3790-E444-9C90-6BF5633E17FB}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -1409,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F821AE-14EF-9447-94FD-816F31696438}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1582,9 +1582,6 @@
       <c r="C12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1596,9 +1593,6 @@
       <c r="C13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1610,9 +1604,6 @@
       <c r="C14" t="s">
         <v>61</v>
       </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1624,9 +1615,6 @@
       <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="D15" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1638,11 +1626,8 @@
       <c r="C16" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -1652,11 +1637,8 @@
       <c r="C17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -1666,11 +1648,8 @@
       <c r="C18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -1680,11 +1659,8 @@
       <c r="C19" t="s">
         <v>76</v>
       </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -1694,11 +1670,8 @@
       <c r="C20" t="s">
         <v>79</v>
       </c>
-      <c r="D20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -1708,11 +1681,8 @@
       <c r="C21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -1722,11 +1692,8 @@
       <c r="C22" t="s">
         <v>83</v>
       </c>
-      <c r="D22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -1736,11 +1703,8 @@
       <c r="C23" t="s">
         <v>84</v>
       </c>
-      <c r="D23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -1750,11 +1714,8 @@
       <c r="C24" t="s">
         <v>85</v>
       </c>
-      <c r="D24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>110</v>
       </c>
@@ -1764,11 +1725,8 @@
       <c r="C25" t="s">
         <v>86</v>
       </c>
-      <c r="D25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -1777,9 +1735,6 @@
       </c>
       <c r="C26" t="s">
         <v>87</v>
-      </c>
-      <c r="D26" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
YTI-1048: Bugfixes to codescheme language impl and related integration test content fixes.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62E2618-C61F-1644-BD82-9B7DE3F8E372}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB11F27-2D9D-F343-8B4B-6D6675F59B39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="31540" activeTab="3" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="31540" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="134">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>Extensions_test</t>
+  </si>
+  <si>
+    <t>LANGUAGECODE</t>
+  </si>
+  <si>
+    <t>fi;sv;en</t>
   </si>
 </sst>
 </file>
@@ -776,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3255037-6CC6-5342-A480-CDB6C5B76D51}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,10 +797,11 @@
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -820,19 +827,22 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>127</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -851,16 +861,19 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1409,7 +1422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F821AE-14EF-9447-94FD-816F31696438}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
YTI-1004: Import support for organization columns in codescheme import. Bugfixing integration tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB11F27-2D9D-F343-8B4B-6D6675F59B39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701AEA7B-94BB-A042-8D97-D70E057319E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="31540" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="136">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>fi;sv;en</t>
+  </si>
+  <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>d9c76d52-03d3-4480-8c2c-b66e6d9c57f2</t>
   </si>
 </sst>
 </file>
@@ -782,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3255037-6CC6-5342-A480-CDB6C5B76D51}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,12 +802,13 @@
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -824,25 +831,28 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>132</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>127</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -859,21 +869,24 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfix to earlier integration test data that was faulty.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
+++ b/src/test/resources/codeschemes/v1_extensionscheme_test.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuukka\git\yti-codelist-content-intake-service\src\test\resources\codeschemes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2747DE28-C9A7-4E5F-AB9E-2DCA2123E226}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501ADCE9-A9E0-2A46-A871-C16951FDD865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
     <sheet name="Codes_exttest1" sheetId="2" r:id="rId2"/>
-    <sheet name="ExtensionSchemes_exttest1" sheetId="3" r:id="rId3"/>
-    <sheet name="Extensions_test" sheetId="4" r:id="rId4"/>
+    <sheet name="Extensions_exttest1" sheetId="3" r:id="rId3"/>
+    <sheet name="Members_test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="145">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -405,9 +405,6 @@
     <t>ORDER</t>
   </si>
   <si>
-    <t>EXTENSIONSCHEMESSHEET</t>
-  </si>
-  <si>
     <t>CODESSHEET</t>
   </si>
   <si>
@@ -417,12 +414,6 @@
     <t>Codes_exttest1</t>
   </si>
   <si>
-    <t>ExtensionSchemes_exttest1</t>
-  </si>
-  <si>
-    <t>Extensions_test</t>
-  </si>
-  <si>
     <t>LANGUAGECODE</t>
   </si>
   <si>
@@ -436,16 +427,58 @@
   </si>
   <si>
     <t>INFORMATIONDOMAIN</t>
+  </si>
+  <si>
+    <t>MEMBERSSHEET</t>
+  </si>
+  <si>
+    <t>Members_test</t>
+  </si>
+  <si>
+    <t>code:testcode01</t>
+  </si>
+  <si>
+    <t>code:testcode02</t>
+  </si>
+  <si>
+    <t>code:testcode03</t>
+  </si>
+  <si>
+    <t>code:testcode04</t>
+  </si>
+  <si>
+    <t>code:testcode05</t>
+  </si>
+  <si>
+    <t>code:testcode06</t>
+  </si>
+  <si>
+    <t>code:testcode07</t>
+  </si>
+  <si>
+    <t>code:testcode08</t>
+  </si>
+  <si>
+    <t>code:testcode09</t>
+  </si>
+  <si>
+    <t>Extensions_exttest1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -790,25 +823,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3255037-6CC6-5342-A480-CDB6C5B76D51}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.625" customWidth="1"/>
-    <col min="5" max="5" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.875" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" customWidth="1"/>
     <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -831,13 +864,13 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K1" t="s">
         <v>19</v>
@@ -846,13 +879,13 @@
         <v>20</v>
       </c>
       <c r="M1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" t="s">
         <v>126</v>
       </c>
-      <c r="N1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -869,13 +902,13 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>25</v>
@@ -884,10 +917,10 @@
         <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -904,13 +937,13 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -944,7 +977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -961,7 +994,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -978,7 +1011,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -995,7 +1028,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1012,7 +1045,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1029,7 +1062,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1046,7 +1079,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1063,7 +1096,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1080,7 +1113,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1097,7 +1130,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1114,7 +1147,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1131,7 +1164,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1148,7 +1181,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1165,7 +1198,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -1182,7 +1215,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1199,7 +1232,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1216,7 +1249,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -1233,7 +1266,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1250,7 +1283,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1267,7 +1300,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1284,7 +1317,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -1301,7 +1334,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -1318,7 +1351,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -1335,7 +1368,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -1361,20 +1394,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4460C0-3790-E444-9C90-6BF5633E17FB}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1397,10 +1430,10 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1423,7 +1456,7 @@
         <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1436,18 +1469,18 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1461,7 +1494,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1472,7 +1505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1483,10 +1516,10 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1497,10 +1530,10 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1511,10 +1544,10 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -1525,10 +1558,10 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -1539,10 +1572,10 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -1553,10 +1586,10 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1567,10 +1600,10 @@
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -1581,10 +1614,10 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -1595,10 +1628,10 @@
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -1609,7 +1642,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -1620,7 +1653,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -1631,7 +1664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1642,7 +1675,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -1653,7 +1686,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1664,7 +1697,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -1675,7 +1708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1686,7 +1719,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -1697,7 +1730,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -1708,7 +1741,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -1719,7 +1752,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>107</v>
       </c>
@@ -1730,7 +1763,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1741,7 +1774,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -1752,7 +1785,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -1764,6 +1797,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>